<commit_message>
Add comments, Edit variable names, Add settings sheet
</commit_message>
<xml_diff>
--- a/customDiceOutcomes.xlsx
+++ b/customDiceOutcomes.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thias\OneDrive\Dokumenter\GitHub\read-excel-files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D881B464-9794-4227-9072-20F2A725C2E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2F49F4D-6213-42A1-B84E-1E2EF06E260D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="diceOutcomes" sheetId="1" r:id="rId1"/>
+    <sheet name="settings" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="27">
   <si>
     <t>Dierolls</t>
   </si>
@@ -103,6 +104,15 @@
   </si>
   <si>
     <t>(The outcome-, and GoTo-cells are merged for visual reasons, but they are 'really' placed in the same row as their min-cell.)</t>
+  </si>
+  <si>
+    <t>Maximum number of rolls, without user input:</t>
+  </si>
+  <si>
+    <t>Setting</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
 </sst>
 </file>
@@ -749,7 +759,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
@@ -785,6 +795,18 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -794,6 +816,24 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="19" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -803,36 +843,13 @@
     <xf numFmtId="0" fontId="0" fillId="35" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="34" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1195,8 +1212,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5:D6"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D37" sqref="D37:D38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1229,12 +1246,10 @@
       <c r="B2" s="4">
         <v>1</v>
       </c>
-      <c r="C2" s="29" t="s">
+      <c r="C2" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="29">
-        <v>2</v>
-      </c>
+      <c r="D2" s="23"/>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
@@ -1243,22 +1258,22 @@
       <c r="B3" s="4">
         <v>10</v>
       </c>
-      <c r="C3" s="29"/>
-      <c r="D3" s="29"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="23"/>
     </row>
     <row r="4" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="6"/>
       <c r="B4" s="15"/>
       <c r="C4" s="14"/>
       <c r="D4" s="21"/>
-      <c r="F4" s="33" t="s">
+      <c r="F4" s="30" t="s">
         <v>21</v>
       </c>
-      <c r="G4" s="34"/>
-      <c r="H4" s="34"/>
-      <c r="I4" s="34"/>
-      <c r="J4" s="34"/>
-      <c r="K4" s="35"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="31"/>
+      <c r="I4" s="31"/>
+      <c r="J4" s="31"/>
+      <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1267,16 +1282,16 @@
       <c r="B5" s="11">
         <v>11</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="D5" s="29"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="37"/>
-      <c r="J5" s="37"/>
-      <c r="K5" s="38"/>
+      <c r="D5" s="23"/>
+      <c r="F5" s="33"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="35"/>
     </row>
     <row r="6" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
@@ -1285,8 +1300,8 @@
       <c r="B6" s="12">
         <v>20</v>
       </c>
-      <c r="C6" s="29"/>
-      <c r="D6" s="29"/>
+      <c r="C6" s="23"/>
+      <c r="D6" s="23"/>
       <c r="F6" s="10"/>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
@@ -1307,10 +1322,10 @@
       <c r="B8" s="13">
         <v>21</v>
       </c>
-      <c r="C8" s="29" t="s">
+      <c r="C8" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="D8" s="29"/>
+      <c r="D8" s="23"/>
       <c r="F8" s="5" t="s">
         <v>14</v>
       </c>
@@ -1327,28 +1342,28 @@
       <c r="B9" s="13">
         <v>30</v>
       </c>
-      <c r="C9" s="29"/>
-      <c r="D9" s="29"/>
-      <c r="F9" s="30" t="s">
+      <c r="C9" s="23"/>
+      <c r="D9" s="23"/>
+      <c r="F9" s="24" t="s">
         <v>15</v>
       </c>
-      <c r="G9" s="31"/>
-      <c r="H9" s="31"/>
-      <c r="I9" s="31"/>
-      <c r="J9" s="31"/>
-      <c r="K9" s="32"/>
+      <c r="G9" s="25"/>
+      <c r="H9" s="25"/>
+      <c r="I9" s="25"/>
+      <c r="J9" s="25"/>
+      <c r="K9" s="26"/>
     </row>
     <row r="10" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="6"/>
       <c r="B10" s="22"/>
       <c r="C10" s="14"/>
       <c r="D10" s="21"/>
-      <c r="F10" s="23"/>
-      <c r="G10" s="24"/>
-      <c r="H10" s="24"/>
-      <c r="I10" s="24"/>
-      <c r="J10" s="24"/>
-      <c r="K10" s="25"/>
+      <c r="F10" s="27"/>
+      <c r="G10" s="28"/>
+      <c r="H10" s="28"/>
+      <c r="I10" s="28"/>
+      <c r="J10" s="28"/>
+      <c r="K10" s="29"/>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -1357,16 +1372,16 @@
       <c r="B11" s="13">
         <v>31</v>
       </c>
-      <c r="C11" s="29" t="s">
+      <c r="C11" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="D11" s="29"/>
-      <c r="F11" s="23"/>
-      <c r="G11" s="24"/>
-      <c r="H11" s="24"/>
-      <c r="I11" s="24"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="25"/>
+      <c r="D11" s="23"/>
+      <c r="F11" s="27"/>
+      <c r="G11" s="28"/>
+      <c r="H11" s="28"/>
+      <c r="I11" s="28"/>
+      <c r="J11" s="28"/>
+      <c r="K11" s="29"/>
     </row>
     <row r="12" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
@@ -1375,28 +1390,28 @@
       <c r="B12" s="13">
         <v>40</v>
       </c>
-      <c r="C12" s="29"/>
-      <c r="D12" s="29"/>
-      <c r="F12" s="23" t="s">
+      <c r="C12" s="23"/>
+      <c r="D12" s="23"/>
+      <c r="F12" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="G12" s="24"/>
-      <c r="H12" s="24"/>
-      <c r="I12" s="24"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="25"/>
+      <c r="G12" s="28"/>
+      <c r="H12" s="28"/>
+      <c r="I12" s="28"/>
+      <c r="J12" s="28"/>
+      <c r="K12" s="29"/>
     </row>
     <row r="13" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="6"/>
       <c r="B13" s="22"/>
       <c r="C13" s="14"/>
       <c r="D13" s="21"/>
-      <c r="F13" s="23"/>
-      <c r="G13" s="24"/>
-      <c r="H13" s="24"/>
-      <c r="I13" s="24"/>
-      <c r="J13" s="24"/>
-      <c r="K13" s="25"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+      <c r="I13" s="28"/>
+      <c r="J13" s="28"/>
+      <c r="K13" s="29"/>
     </row>
     <row r="14" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
@@ -1405,16 +1420,16 @@
       <c r="B14" s="13">
         <v>41</v>
       </c>
-      <c r="C14" s="29" t="s">
+      <c r="C14" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="D14" s="29"/>
-      <c r="F14" s="23"/>
-      <c r="G14" s="24"/>
-      <c r="H14" s="24"/>
-      <c r="I14" s="24"/>
-      <c r="J14" s="24"/>
-      <c r="K14" s="25"/>
+      <c r="D14" s="23"/>
+      <c r="F14" s="27"/>
+      <c r="G14" s="28"/>
+      <c r="H14" s="28"/>
+      <c r="I14" s="28"/>
+      <c r="J14" s="28"/>
+      <c r="K14" s="29"/>
     </row>
     <row r="15" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
@@ -1423,28 +1438,28 @@
       <c r="B15" s="13">
         <v>50</v>
       </c>
-      <c r="C15" s="29"/>
-      <c r="D15" s="29"/>
-      <c r="F15" s="23" t="s">
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="F15" s="27" t="s">
         <v>23</v>
       </c>
-      <c r="G15" s="24"/>
-      <c r="H15" s="24"/>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="25"/>
+      <c r="G15" s="28"/>
+      <c r="H15" s="28"/>
+      <c r="I15" s="28"/>
+      <c r="J15" s="28"/>
+      <c r="K15" s="29"/>
     </row>
     <row r="16" spans="1:11" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="6"/>
       <c r="B16" s="22"/>
       <c r="C16" s="14"/>
       <c r="D16" s="21"/>
-      <c r="F16" s="26"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
-      <c r="J16" s="27"/>
-      <c r="K16" s="28"/>
+      <c r="F16" s="36"/>
+      <c r="G16" s="37"/>
+      <c r="H16" s="37"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="37"/>
+      <c r="K16" s="38"/>
     </row>
     <row r="17" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
@@ -1453,10 +1468,10 @@
       <c r="B17" s="13">
         <v>51</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D17" s="29"/>
+      <c r="D17" s="23"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
@@ -1465,8 +1480,8 @@
       <c r="B18" s="13">
         <v>60</v>
       </c>
-      <c r="C18" s="29"/>
-      <c r="D18" s="29"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="23"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" s="6"/>
@@ -1481,10 +1496,10 @@
       <c r="B20" s="13">
         <v>61</v>
       </c>
-      <c r="C20" s="29" t="s">
+      <c r="C20" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="29"/>
+      <c r="D20" s="23"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
@@ -1493,8 +1508,8 @@
       <c r="B21" s="13">
         <v>70</v>
       </c>
-      <c r="C21" s="29"/>
-      <c r="D21" s="29"/>
+      <c r="C21" s="23"/>
+      <c r="D21" s="23"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" s="6"/>
@@ -1509,10 +1524,10 @@
       <c r="B23" s="13">
         <v>71</v>
       </c>
-      <c r="C23" s="29" t="s">
+      <c r="C23" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="29"/>
+      <c r="D23" s="23"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" s="2" t="s">
@@ -1521,8 +1536,8 @@
       <c r="B24" s="13">
         <v>80</v>
       </c>
-      <c r="C24" s="29"/>
-      <c r="D24" s="29"/>
+      <c r="C24" s="23"/>
+      <c r="D24" s="23"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" s="6"/>
@@ -1537,10 +1552,10 @@
       <c r="B26" s="13">
         <v>81</v>
       </c>
-      <c r="C26" s="29" t="s">
+      <c r="C26" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="D26" s="29"/>
+      <c r="D26" s="23"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" s="2" t="s">
@@ -1549,8 +1564,8 @@
       <c r="B27" s="13">
         <v>90</v>
       </c>
-      <c r="C27" s="29"/>
-      <c r="D27" s="29"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" s="6"/>
@@ -1565,10 +1580,10 @@
       <c r="B29" s="13">
         <v>91</v>
       </c>
-      <c r="C29" s="29" t="s">
+      <c r="C29" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="D29" s="29"/>
+      <c r="D29" s="23"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
@@ -1577,8 +1592,8 @@
       <c r="B30" s="13">
         <v>100</v>
       </c>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" s="7"/>
@@ -1611,10 +1626,10 @@
       <c r="B34" s="4">
         <v>5</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D34" s="29"/>
+      <c r="D34" s="23"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
@@ -1623,8 +1638,8 @@
       <c r="B35" s="4">
         <v>10</v>
       </c>
-      <c r="C35" s="29"/>
-      <c r="D35" s="29"/>
+      <c r="C35" s="23"/>
+      <c r="D35" s="23"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" s="6"/>
@@ -1639,10 +1654,10 @@
       <c r="B37" s="11">
         <v>11</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="D37" s="29"/>
+      <c r="D37" s="23"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
@@ -1651,8 +1666,8 @@
       <c r="B38" s="12">
         <v>20</v>
       </c>
-      <c r="C38" s="29"/>
-      <c r="D38" s="29"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B39" s="1"/>
@@ -1735,6 +1750,14 @@
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C2:C3"/>
     <mergeCell ref="C34:C35"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="D8:D9"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="F12:K14"/>
+    <mergeCell ref="F15:K16"/>
+    <mergeCell ref="D34:D35"/>
     <mergeCell ref="C37:C38"/>
     <mergeCell ref="C23:C24"/>
     <mergeCell ref="C26:C27"/>
@@ -1744,14 +1767,6 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C17:C18"/>
     <mergeCell ref="C20:C21"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="D8:D9"/>
-    <mergeCell ref="D11:D12"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="F12:K14"/>
-    <mergeCell ref="F15:K16"/>
-    <mergeCell ref="D34:D35"/>
     <mergeCell ref="D37:D38"/>
     <mergeCell ref="D17:D18"/>
     <mergeCell ref="D20:D21"/>
@@ -1763,4 +1778,49 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1BA7DD6E-E73A-4D62-A2FD-C7B3FD3B5EC0}">
+  <dimension ref="A1:C3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="21.44140625" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="40" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="39">
+        <v>20</v>
+      </c>
+      <c r="C2" s="41"/>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="40"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="41"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="B2:B3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>